<commit_message>
Added sGroupArray to figure out slabs. Also filled out more of the Routine/Contrast tab
</commit_message>
<xml_diff>
--- a/dcm2prot/dcm2prot parameters.xlsx
+++ b/dcm2prot/dcm2prot parameters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Dropbox\Personal\Other\dcm2prot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\Visual Studio 2010\Projects\dcm2prot\dcm2prot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="psir" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,10 @@
     <sheet name="localizer" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="da0c86252d0dba30a740b056c61d23040b03089f2d05df7a707bf7c5f33a68d2" localSheetId="1">cv_nav!$F$240</definedName>
+    <definedName name="da0c86252d0dba30a740b056c61d23046a41046a33d5d2ed9766fb9b07096a19" localSheetId="1">cv_nav!$F$241</definedName>
+    <definedName name="da0c86252d0dba30a740b056c61d23049abca77c98654bc041cc284335388c91" localSheetId="1">cv_nav!$F$238</definedName>
+    <definedName name="da0c86252d0dba30a740b056c61d2304bcd9e20fb2ae7a8107b514bc71c62a86" localSheetId="1">cv_nav!$F$239</definedName>
     <definedName name="f179de84294fd549821135bd5a7d239a4287cccb3221b15f07c7368f864fe34a" localSheetId="0">psir!$I$235</definedName>
     <definedName name="f179de84294fd549821135bd5a7d239a4b2834abc1975e3764a3c9fb1321e7f3" localSheetId="0">psir!$I$238</definedName>
     <definedName name="f179de84294fd549821135bd5a7d239a5a678bc9c59f232dc3495eaaa2c4643b" localSheetId="0">psir!$I$237</definedName>
@@ -70,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3052" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3057" uniqueCount="873">
   <si>
     <t>### ASCCONV BEGIN ###</t>
   </si>
@@ -2818,6 +2822,81 @@
   </si>
   <si>
     <t>Composing.Distortion Corr</t>
+  </si>
+  <si>
+    <r>
+      <t>SLICE_SELECTIVE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>VOLUME_SELECTIVE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INVERSION_OFF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T2_SELECTIVE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>VOLUME_SELECTIVE_DIR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3179,9 +3258,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M393"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A201" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J218" sqref="J218"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6637,16 +6716,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C521"/>
+  <dimension ref="A1:G521"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="E240" sqref="E240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.140625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="6" max="6" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -8456,7 +8536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>634</v>
       </c>
@@ -8467,7 +8547,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>635</v>
       </c>
@@ -8478,7 +8558,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>636</v>
       </c>
@@ -8486,7 +8566,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>637</v>
       </c>
@@ -8497,7 +8577,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>638</v>
       </c>
@@ -8508,7 +8588,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>639</v>
       </c>
@@ -8519,7 +8599,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>640</v>
       </c>
@@ -8530,7 +8610,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>641</v>
       </c>
@@ -8541,7 +8621,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>200</v>
       </c>
@@ -8549,7 +8629,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>201</v>
       </c>
@@ -8557,7 +8637,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>202</v>
       </c>
@@ -8565,7 +8645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>204</v>
       </c>
@@ -8573,7 +8653,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>205</v>
       </c>
@@ -8583,32 +8663,48 @@
       <c r="C237" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F237" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="G237" s="5"/>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>206</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F238" s="4" t="s">
+        <v>869</v>
+      </c>
+      <c r="G238" s="5"/>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>207</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F239" s="4" t="s">
+        <v>870</v>
+      </c>
+      <c r="G239" s="5"/>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>208</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F240" s="4" t="s">
+        <v>871</v>
+      </c>
+      <c r="G240" s="5"/>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>209</v>
       </c>
@@ -8618,8 +8714,12 @@
       <c r="C241" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F241" s="4" t="s">
+        <v>872</v>
+      </c>
+      <c r="G241" s="5"/>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>210</v>
       </c>
@@ -8627,7 +8727,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>211</v>
       </c>
@@ -8635,7 +8735,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>212</v>
       </c>
@@ -8646,7 +8746,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>213</v>
       </c>
@@ -8654,7 +8754,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>214</v>
       </c>
@@ -8662,7 +8762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>215</v>
       </c>
@@ -8670,7 +8770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>216</v>
       </c>
@@ -8678,7 +8778,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>217</v>
       </c>
@@ -8686,7 +8786,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>218</v>
       </c>
@@ -8694,7 +8794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>219</v>
       </c>
@@ -8702,7 +8802,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>220</v>
       </c>
@@ -8710,7 +8810,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>221</v>
       </c>
@@ -8718,7 +8818,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>222</v>
       </c>
@@ -8726,7 +8826,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>223</v>
       </c>
@@ -8734,7 +8834,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>224</v>
       </c>
@@ -10874,8 +10974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C383"/>
   <sheetViews>
-    <sheetView topLeftCell="A366" workbookViewId="0">
-      <selection activeCell="A215" sqref="A215"/>
+    <sheetView topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="A184" sqref="A184:B188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13946,8 +14046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C462"/>
   <sheetViews>
-    <sheetView topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="A217" sqref="A217"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="A190" sqref="A190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17658,8 +17758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C493"/>
   <sheetViews>
-    <sheetView topLeftCell="A261" workbookViewId="0">
-      <selection activeCell="B281" sqref="A281:B281"/>
+    <sheetView topLeftCell="A333" workbookViewId="0">
+      <selection activeCell="B346" sqref="B346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Still filling out the tabs...
</commit_message>
<xml_diff>
--- a/dcm2prot/dcm2prot parameters.xlsx
+++ b/dcm2prot/dcm2prot parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="psir" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3057" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3058" uniqueCount="874">
   <si>
     <t>### ASCCONV BEGIN ###</t>
   </si>
@@ -2897,6 +2897,9 @@
       </rPr>
       <t> </t>
     </r>
+  </si>
+  <si>
+    <t>Fat Suppression…?</t>
   </si>
 </sst>
 </file>
@@ -3258,9 +3261,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M393"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A164" sqref="A164"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D195" sqref="D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4870,6 +4873,9 @@
       <c r="B187" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="D187" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
@@ -4936,7 +4942,7 @@
         <v>145</v>
       </c>
       <c r="D194" t="s">
-        <v>736</v>
+        <v>873</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
@@ -6718,8 +6724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G521"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
-      <selection activeCell="E240" sqref="E240"/>
+    <sheetView topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="C241" sqref="C241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10975,7 +10981,7 @@
   <dimension ref="A2:C383"/>
   <sheetViews>
     <sheetView topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="A184" sqref="A184:B188"/>
+      <selection activeCell="B190" sqref="A190:B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14047,7 +14053,7 @@
   <dimension ref="A1:C462"/>
   <sheetViews>
     <sheetView topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="A190" sqref="A190"/>
+      <selection activeCell="A188" sqref="A188:B188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17758,8 +17764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C493"/>
   <sheetViews>
-    <sheetView topLeftCell="A333" workbookViewId="0">
-      <selection activeCell="B346" sqref="B346"/>
+    <sheetView topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="A246" sqref="A246:B246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>